<commit_message>
added in exception handling and an error log
</commit_message>
<xml_diff>
--- a/generated/output 02-17-2022.xlsx
+++ b/generated/output 02-17-2022.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pruit\Desktop\dev\senior-project\generated\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA3456F-0B65-4205-BA3E-01324A591CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="2160" windowWidth="28680" windowHeight="15340" tabRatio="755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="MaddenCo Daily Data 02-17-2022" sheetId="1" r:id="rId1"/>
@@ -19,12 +13,12 @@
     <sheet name="MaddenCo All Count 02-17-2022" sheetId="4" r:id="rId4"/>
     <sheet name="MaddenCo Total Count 02-17-2022" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="111">
   <si>
     <t>Date Created</t>
   </si>
@@ -362,8 +356,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,14 +487,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -547,7 +533,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,27 +565,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -631,24 +599,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -824,27 +774,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7265625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -873,7 +821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>20220106</v>
       </c>
@@ -902,7 +850,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>20220106</v>
       </c>
@@ -931,7 +879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>20220106</v>
       </c>
@@ -960,7 +908,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>20220106</v>
       </c>
@@ -989,7 +937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>20220106</v>
       </c>
@@ -1018,7 +966,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>20220106</v>
       </c>
@@ -1047,7 +995,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>20220106</v>
       </c>
@@ -1076,7 +1024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>20220106</v>
       </c>
@@ -1105,7 +1053,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>20220106</v>
       </c>
@@ -1134,7 +1082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>20220106</v>
       </c>
@@ -1163,7 +1111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>20220106</v>
       </c>
@@ -1192,7 +1140,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>20220106</v>
       </c>
@@ -1221,7 +1169,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>20220106</v>
       </c>
@@ -1250,7 +1198,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>20220106</v>
       </c>
@@ -1279,7 +1227,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>20220106</v>
       </c>
@@ -1308,7 +1256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>20220106</v>
       </c>
@@ -1337,7 +1285,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>20220106</v>
       </c>
@@ -1366,7 +1314,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>20220106</v>
       </c>
@@ -1395,7 +1343,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>20220106</v>
       </c>
@@ -1424,7 +1372,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>20220106</v>
       </c>
@@ -1453,7 +1401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20220106</v>
       </c>
@@ -1482,7 +1430,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>20220106</v>
       </c>
@@ -1511,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>20220106</v>
       </c>
@@ -1540,7 +1488,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>20220106</v>
       </c>
@@ -1569,7 +1517,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>20220106</v>
       </c>
@@ -1598,7 +1546,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>20220106</v>
       </c>
@@ -1627,7 +1575,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>20220106</v>
       </c>
@@ -1656,7 +1604,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>20220106</v>
       </c>
@@ -1685,7 +1633,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>20220106</v>
       </c>
@@ -1714,7 +1662,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>20220106</v>
       </c>
@@ -1743,7 +1691,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>20220106</v>
       </c>
@@ -1772,7 +1720,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>20220106</v>
       </c>
@@ -1801,7 +1749,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>20220106</v>
       </c>
@@ -1830,7 +1778,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>20220106</v>
       </c>
@@ -1859,7 +1807,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>20220106</v>
       </c>
@@ -1888,7 +1836,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>20220106</v>
       </c>
@@ -1917,7 +1865,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>20220106</v>
       </c>
@@ -1946,7 +1894,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>20220106</v>
       </c>
@@ -1975,7 +1923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>20220106</v>
       </c>
@@ -2004,7 +1952,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>20220106</v>
       </c>
@@ -2033,7 +1981,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>20220106</v>
       </c>
@@ -2062,7 +2010,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>20220106</v>
       </c>
@@ -2091,7 +2039,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>20220106</v>
       </c>
@@ -2120,7 +2068,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>20220106</v>
       </c>
@@ -2149,7 +2097,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>20220106</v>
       </c>
@@ -2178,7 +2126,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>20220106</v>
       </c>
@@ -2213,25 +2161,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7265625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2260,7 +2208,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>20220106</v>
       </c>
@@ -2289,7 +2237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>20220106</v>
       </c>
@@ -2318,7 +2266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>20220105</v>
       </c>
@@ -2347,7 +2295,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>20220106</v>
       </c>
@@ -2376,7 +2324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>20220106</v>
       </c>
@@ -2405,7 +2353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>20220106</v>
       </c>
@@ -2434,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>20220106</v>
       </c>
@@ -2463,7 +2411,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>20220106</v>
       </c>
@@ -2492,7 +2440,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>20220106</v>
       </c>
@@ -2521,7 +2469,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>20220106</v>
       </c>
@@ -2550,7 +2498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>20220106</v>
       </c>
@@ -2579,7 +2527,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>20220106</v>
       </c>
@@ -2608,7 +2556,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>20220106</v>
       </c>
@@ -2637,7 +2585,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>20220106</v>
       </c>
@@ -2666,7 +2614,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>20220106</v>
       </c>
@@ -2695,7 +2643,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>20220106</v>
       </c>
@@ -2724,7 +2672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>20220106</v>
       </c>
@@ -2753,7 +2701,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>20220106</v>
       </c>
@@ -2782,7 +2730,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>20220106</v>
       </c>
@@ -2811,7 +2759,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>20220105</v>
       </c>
@@ -2840,7 +2788,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20220106</v>
       </c>
@@ -2869,7 +2817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>20220106</v>
       </c>
@@ -2898,7 +2846,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>20220106</v>
       </c>
@@ -2927,7 +2875,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>20220106</v>
       </c>
@@ -2956,7 +2904,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>20220106</v>
       </c>
@@ -2985,7 +2933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>20220105</v>
       </c>
@@ -3014,7 +2962,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>20220105</v>
       </c>
@@ -3043,7 +2991,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>20220106</v>
       </c>
@@ -3072,7 +3020,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>20220106</v>
       </c>
@@ -3101,7 +3049,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>20220106</v>
       </c>
@@ -3130,7 +3078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>20220106</v>
       </c>
@@ -3159,7 +3107,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>20220106</v>
       </c>
@@ -3188,7 +3136,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>20220105</v>
       </c>
@@ -3217,7 +3165,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>20220106</v>
       </c>
@@ -3246,7 +3194,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>20220106</v>
       </c>
@@ -3275,7 +3223,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>20211029</v>
       </c>
@@ -3304,7 +3252,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>20220106</v>
       </c>
@@ -3333,7 +3281,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>20211019</v>
       </c>
@@ -3362,7 +3310,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>20220106</v>
       </c>
@@ -3391,7 +3339,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>20220106</v>
       </c>
@@ -3420,7 +3368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>20220106</v>
       </c>
@@ -3449,7 +3397,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>20220106</v>
       </c>
@@ -3478,7 +3426,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>20211111</v>
       </c>
@@ -3507,7 +3455,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>20220104</v>
       </c>
@@ -3536,7 +3484,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>20220106</v>
       </c>
@@ -3565,7 +3513,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>20220104</v>
       </c>
@@ -3594,7 +3542,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>20220106</v>
       </c>
@@ -3623,7 +3571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>20220104</v>
       </c>
@@ -3652,7 +3600,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>20220104</v>
       </c>
@@ -3681,7 +3629,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>20220105</v>
       </c>
@@ -3710,7 +3658,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>20220106</v>
       </c>
@@ -3739,7 +3687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>20220106</v>
       </c>
@@ -3768,7 +3716,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>20220106</v>
       </c>
@@ -3797,7 +3745,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>20220106</v>
       </c>
@@ -3826,7 +3774,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>20211220</v>
       </c>
@@ -3855,7 +3803,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>20211213</v>
       </c>
@@ -3884,7 +3832,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>20220105</v>
       </c>
@@ -3913,7 +3861,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>20211215</v>
       </c>
@@ -3942,7 +3890,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>20220106</v>
       </c>
@@ -3971,7 +3919,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>20220106</v>
       </c>
@@ -4000,7 +3948,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>20211206</v>
       </c>
@@ -4029,7 +3977,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>20211219</v>
       </c>
@@ -4058,7 +4006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>20220105</v>
       </c>
@@ -4087,7 +4035,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>20211217</v>
       </c>
@@ -4116,7 +4064,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>20211101</v>
       </c>
@@ -4145,7 +4093,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>20211217</v>
       </c>
@@ -4174,7 +4122,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>20220103</v>
       </c>
@@ -4203,7 +4151,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>20220104</v>
       </c>
@@ -4232,7 +4180,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>20220106</v>
       </c>
@@ -4261,7 +4209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>20211217</v>
       </c>
@@ -4290,7 +4238,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9">
       <c r="A72" s="1">
         <v>20220105</v>
       </c>
@@ -4319,7 +4267,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9">
       <c r="A73" s="1">
         <v>20220105</v>
       </c>
@@ -4348,7 +4296,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9">
       <c r="A74" s="1">
         <v>20220105</v>
       </c>
@@ -4377,7 +4325,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9">
       <c r="A75" s="1">
         <v>20220103</v>
       </c>
@@ -4406,7 +4354,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9">
       <c r="A76" s="1">
         <v>20220105</v>
       </c>
@@ -4435,7 +4383,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9">
       <c r="A77" s="1">
         <v>20220106</v>
       </c>
@@ -4464,7 +4412,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9">
       <c r="A78" s="1">
         <v>20220106</v>
       </c>
@@ -4493,7 +4441,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9">
       <c r="A79" s="1">
         <v>20220105</v>
       </c>
@@ -4522,7 +4470,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9">
       <c r="A80" s="1">
         <v>20220105</v>
       </c>
@@ -4551,7 +4499,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9">
       <c r="A81" s="1">
         <v>20220105</v>
       </c>
@@ -4586,24 +4534,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.7265625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="B1" s="7">
         <v>142</v>
       </c>
@@ -4626,7 +4574,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>107</v>
       </c>
@@ -4652,7 +4600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>108</v>
       </c>
@@ -4678,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>109</v>
       </c>
@@ -4704,7 +4652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>110</v>
       </c>
@@ -4736,24 +4684,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.7265625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="B1" s="7">
         <v>142</v>
       </c>
@@ -4776,7 +4724,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>107</v>
       </c>
@@ -4802,7 +4750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>108</v>
       </c>
@@ -4828,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>109</v>
       </c>
@@ -4854,7 +4802,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>110</v>
       </c>
@@ -4886,26 +4834,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25.7265625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="25.7265625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="B1" s="7">
         <v>142</v>
       </c>
@@ -4928,7 +4874,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="8" t="s">
         <v>107</v>
       </c>
@@ -4954,7 +4900,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>108</v>
       </c>
@@ -4980,7 +4926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>109</v>
       </c>
@@ -5006,7 +4952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="8" t="s">
         <v>110</v>
       </c>

</xml_diff>